<commit_message>
Various updates, including: - Updating SMD function - Adding QWK function - Updating metrics helper function - Adding subgroup SMD function - Updating tests
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval.xlsx
+++ b/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,71 +12,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>h_mean</t>
-  </si>
-  <si>
-    <t>h_sd</t>
-  </si>
-  <si>
-    <t>h_min</t>
-  </si>
-  <si>
-    <t>h_max</t>
-  </si>
-  <si>
-    <t>sys_mean</t>
-  </si>
-  <si>
-    <t>sys_sd</t>
-  </si>
-  <si>
-    <t>sys_min</t>
-  </si>
-  <si>
-    <t>sys_max</t>
-  </si>
-  <si>
-    <t>corr</t>
-  </si>
-  <si>
-    <t>wtkappa</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>kappa</t>
-  </si>
-  <si>
-    <t>exact_agr</t>
-  </si>
-  <si>
-    <t>adj_agr</t>
-  </si>
-  <si>
-    <t>SMD</t>
-  </si>
-  <si>
-    <t>RMSE</t>
-  </si>
-  <si>
-    <t>scale</t>
-  </si>
-  <si>
-    <t>scale_trim</t>
-  </si>
-  <si>
-    <t>scale_trim_round</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,63 +366,99 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" s="1" t="s"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>h_mean</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>h_sd</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>h_min</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>h_max</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>sys_mean</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>sys_sd</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>sys_min</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>sys_max</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>corr</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>wtkappa</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>R2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>kappa</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>exact_agr</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>adj_agr</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>SMD</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>RMSE</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>17</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>scale</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>200</v>
@@ -520,7 +491,7 @@
         <v>0.7801773732608226</v>
       </c>
       <c r="L2" t="n">
-        <v>0.782122905027933</v>
+        <v>0.7797696841910529</v>
       </c>
       <c r="M2" t="n">
         <v>0.5493203316759327</v>
@@ -535,15 +506,17 @@
         <v>84.5</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.02324751973535285</v>
+        <v>-0.02351246133036713</v>
       </c>
       <c r="R2" t="n">
         <v>0.6189327249996216</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>18</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>scale_trim</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>200</v>
@@ -576,7 +549,7 @@
         <v>0.7801773732608226</v>
       </c>
       <c r="L3" t="n">
-        <v>0.782122905027933</v>
+        <v>0.7797696841910529</v>
       </c>
       <c r="M3" t="n">
         <v>0.5493203316759327</v>
@@ -591,15 +564,17 @@
         <v>84.5</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02324751973535285</v>
+        <v>-0.02351246133036713</v>
       </c>
       <c r="R3" t="n">
         <v>0.6189327249996216</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>19</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>scale_trim_round</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>200</v>
@@ -632,7 +607,7 @@
         <v>0.7831550493332693</v>
       </c>
       <c r="L4" t="n">
-        <v>0.782122905027933</v>
+        <v>0.7821229050279329</v>
       </c>
       <c r="M4" t="n">
         <v>0.5411764705882354</v>
@@ -647,7 +622,7 @@
         <v>99</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.01054416404922412</v>
+        <v>0.01081937260331701</v>
       </c>
       <c r="R4" t="n">
         <v>0.6244997998398398</v>

</xml_diff>

<commit_message>
This commit includes the following updates to address PR comments: - Updates to RST files for documentation - Updates to uility functions to address PR comments - Updates to `analyzer` and `comparer` classes to address PR comments - Minor updates to eval notebooks - Refreshing the test data
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval.xlsx
+++ b/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval.xlsx
@@ -491,7 +491,7 @@
         <v>0.7801773732608226</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7797696841910529</v>
+        <v>0.7808705382933534</v>
       </c>
       <c r="M2" t="n">
         <v>0.5493203316759327</v>
@@ -506,7 +506,7 @@
         <v>84.5</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.02351246133036713</v>
+        <v>0.02351246133036713</v>
       </c>
       <c r="R2" t="n">
         <v>0.6189327249996216</v>
@@ -549,7 +549,7 @@
         <v>0.7801773732608226</v>
       </c>
       <c r="L3" t="n">
-        <v>0.7797696841910529</v>
+        <v>0.7808705382933534</v>
       </c>
       <c r="M3" t="n">
         <v>0.5493203316759327</v>
@@ -564,7 +564,7 @@
         <v>84.5</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.02351246133036713</v>
+        <v>0.02351246133036713</v>
       </c>
       <c r="R3" t="n">
         <v>0.6189327249996216</v>
@@ -607,7 +607,7 @@
         <v>0.7831550493332693</v>
       </c>
       <c r="L4" t="n">
-        <v>0.7821229050279329</v>
+        <v>0.7832122299475502</v>
       </c>
       <c r="M4" t="n">
         <v>0.5411764705882354</v>
@@ -622,7 +622,7 @@
         <v>99</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.01081937260331701</v>
+        <v>-0.01081937260331701</v>
       </c>
       <c r="R4" t="n">
         <v>0.6244997998398398</v>

</xml_diff>

<commit_message>
Copy over test files
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval.xlsx
+++ b/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,6 +12,71 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>h_mean</t>
+  </si>
+  <si>
+    <t>h_sd</t>
+  </si>
+  <si>
+    <t>h_min</t>
+  </si>
+  <si>
+    <t>h_max</t>
+  </si>
+  <si>
+    <t>sys_mean</t>
+  </si>
+  <si>
+    <t>sys_sd</t>
+  </si>
+  <si>
+    <t>sys_min</t>
+  </si>
+  <si>
+    <t>sys_max</t>
+  </si>
+  <si>
+    <t>corr</t>
+  </si>
+  <si>
+    <t>wtkappa</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>kappa</t>
+  </si>
+  <si>
+    <t>exact_agr</t>
+  </si>
+  <si>
+    <t>adj_agr</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>scale_trim</t>
+  </si>
+  <si>
+    <t>scale_trim_round</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,99 +431,63 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>h_mean</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>h_sd</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>h_min</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>h_max</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>sys_mean</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>sys_sd</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>sys_min</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>sys_max</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>corr</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>wtkappa</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>R2</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>kappa</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>exact_agr</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>adj_agr</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>SMD</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>RMSE</t>
-        </is>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>scale</t>
-        </is>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>17</v>
       </c>
       <c r="B2" t="n">
         <v>200</v>
@@ -491,7 +520,7 @@
         <v>0.7801773732608226</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7808705382933534</v>
+        <v>0.782122905027933</v>
       </c>
       <c r="M2" t="n">
         <v>0.5493203316759327</v>
@@ -506,17 +535,15 @@
         <v>84.5</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.02351246133036713</v>
+        <v>0.02324751973535285</v>
       </c>
       <c r="R2" t="n">
         <v>0.6189327249996216</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>scale_trim</t>
-        </is>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>18</v>
       </c>
       <c r="B3" t="n">
         <v>200</v>
@@ -549,7 +576,7 @@
         <v>0.7801773732608226</v>
       </c>
       <c r="L3" t="n">
-        <v>0.7808705382933534</v>
+        <v>0.782122905027933</v>
       </c>
       <c r="M3" t="n">
         <v>0.5493203316759327</v>
@@ -564,17 +591,15 @@
         <v>84.5</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02351246133036713</v>
+        <v>0.02324751973535285</v>
       </c>
       <c r="R3" t="n">
         <v>0.6189327249996216</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>scale_trim_round</t>
-        </is>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>19</v>
       </c>
       <c r="B4" t="n">
         <v>200</v>
@@ -607,7 +632,7 @@
         <v>0.7831550493332693</v>
       </c>
       <c r="L4" t="n">
-        <v>0.7832122299475502</v>
+        <v>0.782122905027933</v>
       </c>
       <c r="M4" t="n">
         <v>0.5411764705882354</v>
@@ -622,7 +647,7 @@
         <v>99</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.01081937260331701</v>
+        <v>-0.01054416404922412</v>
       </c>
       <c r="R4" t="n">
         <v>0.6244997998398398</v>

</xml_diff>

<commit_message>
Updated kappa values in tests
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval.xlsx
+++ b/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval.xlsx
@@ -491,7 +491,7 @@
         <v>0.7801773732608226</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7808705382933534</v>
+        <v>0.7797696841910529</v>
       </c>
       <c r="M2" t="n">
         <v>0.5493203316759327</v>
@@ -549,7 +549,7 @@
         <v>0.7801773732608226</v>
       </c>
       <c r="L3" t="n">
-        <v>0.7808705382933534</v>
+        <v>0.7797696841910529</v>
       </c>
       <c r="M3" t="n">
         <v>0.5493203316759327</v>
@@ -607,7 +607,7 @@
         <v>0.7831550493332693</v>
       </c>
       <c r="L4" t="n">
-        <v>0.7832122299475502</v>
+        <v>0.7821229050279329</v>
       </c>
       <c r="M4" t="n">
         <v>0.5411764705882354</v>

</xml_diff>